<commit_message>
App Finalizado e Funcionando 100%
</commit_message>
<xml_diff>
--- a/diarias.xlsx
+++ b/diarias.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
   <si>
     <t>Data e hora de início</t>
   </si>
@@ -94,6 +94,12 @@
     <t>2025-03-07 06:25:00</t>
   </si>
   <si>
+    <t>2025-03-01 10:35:00</t>
+  </si>
+  <si>
+    <t>2025-03-02 10:37:00</t>
+  </si>
+  <si>
     <t>2025-03-25 19:52:00</t>
   </si>
   <si>
@@ -139,6 +145,12 @@
     <t>2025-03-07 19:25:00</t>
   </si>
   <si>
+    <t>2025-03-01 15:35:00</t>
+  </si>
+  <si>
+    <t>2025-03-02 16:37:00</t>
+  </si>
+  <si>
     <t>Cantina Volpi Lauro</t>
   </si>
   <si>
@@ -169,7 +181,10 @@
     <t>José</t>
   </si>
   <si>
-    <t>94585623502</t>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>1586485914</t>
   </si>
   <si>
     <t>N</t>
@@ -530,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -573,16 +588,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>1234567890</v>
@@ -593,16 +608,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F3">
         <v>1234567899</v>
@@ -613,16 +628,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F4">
         <v>1234567890</v>
@@ -633,16 +648,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F5">
         <v>1234567899</v>
@@ -654,10 +669,10 @@
         <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -665,16 +680,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F6">
         <v>1234567899</v>
@@ -686,10 +701,10 @@
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -697,16 +712,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F7">
         <v>12345678799</v>
@@ -718,10 +733,10 @@
         <v>30</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -729,16 +744,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F8">
         <v>12345678799</v>
@@ -750,10 +765,10 @@
         <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -764,13 +779,13 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F9">
         <v>12345678799</v>
@@ -782,10 +797,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -793,16 +808,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F10">
         <v>12345678799</v>
@@ -814,10 +829,10 @@
         <v>30.08333333333333</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -825,16 +840,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F11">
         <v>1234567899</v>
@@ -846,10 +861,10 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -857,16 +872,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>12345678799</v>
@@ -878,10 +893,10 @@
         <v>45</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -889,16 +904,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F13">
         <v>1234532608</v>
@@ -910,7 +925,7 @@
         <v>50</v>
       </c>
       <c r="I13" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -918,16 +933,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F14">
         <v>52469875612</v>
@@ -939,10 +954,10 @@
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -950,16 +965,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F15">
         <v>1234532608</v>
@@ -971,10 +986,10 @@
         <v>13</v>
       </c>
       <c r="I15" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -982,16 +997,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F16">
         <v>1234532608</v>
@@ -1003,10 +1018,10 @@
         <v>50</v>
       </c>
       <c r="I16" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1014,19 +1029,19 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="F17">
+        <v>94585623502</v>
       </c>
       <c r="G17">
         <v>16</v>
@@ -1035,10 +1050,74 @@
         <v>13</v>
       </c>
       <c r="I17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="J17" t="s">
-        <v>52</v>
+      <c r="F18">
+        <v>1234532608</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+      <c r="H18">
+        <v>50</v>
+      </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19">
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>